<commit_message>
more cases for GAMS commands
</commit_message>
<xml_diff>
--- a/suppxls/Scen_demo_GAMScode.xlsx
+++ b/suppxls/Scen_demo_GAMScode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75DBDB6-64AD-4351-BB76-C33ED7AB16E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83A165D-038F-4DC0-B43C-25472CFEEADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,24 +55,15 @@
     <t>RFCmd_G</t>
   </si>
   <si>
-    <t>GAMS statement 1</t>
-  </si>
-  <si>
     <t>Written GAMSOPT section</t>
   </si>
   <si>
     <t>RFCmd_Glb</t>
   </si>
   <si>
-    <t>GAMS statement 2</t>
-  </si>
-  <si>
     <t>Written to Global parameters section</t>
   </si>
   <si>
-    <t>GAMS statement 3</t>
-  </si>
-  <si>
     <t>SFCmd_T</t>
   </si>
   <si>
@@ -85,15 +76,9 @@
     <t>SFCmd_B</t>
   </si>
   <si>
-    <t>GAMS statement A</t>
-  </si>
-  <si>
     <t>Bottom of the scen DD file</t>
   </si>
   <si>
-    <t>GAMS statement B</t>
-  </si>
-  <si>
     <t>* --&gt;&gt; Do you want debugging?</t>
   </si>
   <si>
@@ -139,10 +124,25 @@
     <t>*3</t>
   </si>
   <si>
-    <t>~TFM_DINS</t>
-  </si>
-  <si>
-    <t>REG1</t>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>*GAMS statement 1</t>
+  </si>
+  <si>
+    <t>*GAMS statement 2</t>
+  </si>
+  <si>
+    <t>*GAMS statement 3</t>
+  </si>
+  <si>
+    <t>*GAMS statement A</t>
+  </si>
+  <si>
+    <t>*GAMS statement B</t>
   </si>
 </sst>
 </file>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,7 @@
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
         <v>3</v>
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>8</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -627,97 +627,97 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
         <v>10</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -756,10 +756,10 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
@@ -770,10 +770,10 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
@@ -784,10 +784,10 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
@@ -798,10 +798,10 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
@@ -812,10 +812,10 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
@@ -826,10 +826,10 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
@@ -840,10 +840,10 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
@@ -854,10 +854,10 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
@@ -868,10 +868,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
@@ -882,10 +882,10 @@
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
@@ -896,10 +896,10 @@
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
@@ -910,10 +910,10 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
@@ -924,10 +924,10 @@
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
@@ -938,15 +938,15 @@
         <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -985,10 +985,10 @@
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
@@ -999,10 +999,10 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
@@ -1013,10 +1013,10 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
@@ -1027,10 +1027,10 @@
         <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
@@ -1041,10 +1041,10 @@
         <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
@@ -1055,10 +1055,10 @@
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
@@ -1069,10 +1069,10 @@
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
@@ -1083,10 +1083,10 @@
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
@@ -1097,10 +1097,10 @@
         <v>10</v>
       </c>
       <c r="E48" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
@@ -1111,10 +1111,10 @@
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
@@ -1125,10 +1125,10 @@
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
@@ -1139,10 +1139,10 @@
         <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
@@ -1153,10 +1153,10 @@
         <v>14</v>
       </c>
       <c r="E52" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
@@ -1167,10 +1167,10 @@
         <v>15</v>
       </c>
       <c r="E53" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>